<commit_message>
criado o plotly "total de filmes por ano"
</commit_message>
<xml_diff>
--- a/data-raw/siglas_moedas_paises.xlsx
+++ b/data-raw/siglas_moedas_paises.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Planilha1!$A$1:$D$250</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Planilha1!$A$1:$D$249</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="610">
   <si>
     <t xml:space="preserve">pais</t>
   </si>
@@ -1423,427 +1423,430 @@
     <t xml:space="preserve">reunião</t>
   </si>
   <si>
+    <t xml:space="preserve">Reino Unido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Libra esterlina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federação Russa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rublo russo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruanda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Franco ruandês</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RWF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saara Ocidental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St. Helena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Livro de Santa Helena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St. Kitts and Nevis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St. Lucia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">San Marino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">São Pedro e Miquelon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St. Vincent e Granadinas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ilhas Salomão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dólar de Salomão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">samoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samoa Americana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">São Tomé e Príncipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Senegal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sérvia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dinar sérvio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seychelles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rúpia de Seychelles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serra Leoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cingapura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dólar de Cingapura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SGD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eslováquia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coroa eslovaca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eslovenia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tolar Esloveno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Somália</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xelim somali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sudão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Libra sudanesa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sri Lanka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rupia do Sri Lanka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LKR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">camurça</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coroa sueca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suíça</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Franco WIR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suriname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dólar do Suriname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ilhas Svalbard e Jan Mayen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suazilândia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lilangeni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SZL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">República Árabe da Síria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Libra síria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SYP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tadjiquistão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">somoni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TJS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taiwan, Província da China</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Novo dólar de Taiwan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tanzânia, República Unida da</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xelim da Tanzânia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TZS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Territórios Franceses do Sul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">República Tcheca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coroa checa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CZK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tailândia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">baht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timor Leste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Togo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tokelau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tonga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tonga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trinidad e Tobago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dólar de Trinidad e Tobago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tunísia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dinar tunisino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turcomenistão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ilhas Turks e Caicos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turquia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lira Turca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tuvalu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ucrânia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hryvnia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UAH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uruguai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso uruguaio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UYU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso uruguaio em Unidades Indexadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uyi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanuatu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vatu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VUV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cidade do Vaticano Estado da Santa Sé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venezuela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bolivar Venezuelano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VEB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vietnã</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wallis e Futuna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iémen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rial do Iêmen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zâmbia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zimbábue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dólar do Zimbábue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZWD</t>
+  </si>
+  <si>
     <t xml:space="preserve">Romênia</t>
   </si>
   <si>
-    <t xml:space="preserve">Os novos nomes serão comunicados mais tarde</t>
+    <t xml:space="preserve">Leu Romeno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leu Romeno Atual</t>
   </si>
   <si>
     <t xml:space="preserve">RON</t>
   </si>
   <si>
-    <t xml:space="preserve">Reino Unido</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Libra esterlina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GBP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Federação Russa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rublo russo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RUR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ruanda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Franco ruandês</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RWF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saara Ocidental</t>
-  </si>
-  <si>
-    <t xml:space="preserve">St. Helena</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Livro de Santa Helena</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">St. Kitts and Nevis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">St. Lucia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">San Marino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">São Pedro e Miquelon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">St. Vincent e Granadinas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ilhas Salomão</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dólar de Salomão</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">samoa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Samoa Americana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">São Tomé e Príncipe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dobra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Senegal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sérvia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dinar sérvio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RSD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seychelles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rúpia de Seychelles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serra Leoa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SLL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cingapura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dólar de Cingapura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SGD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eslováquia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coroa eslovaca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eslovenia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tolar Esloveno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Somália</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Xelim somali</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sudão</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Libra sudanesa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sri Lanka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rupia do Sri Lanka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LKR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">camurça</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coroa sueca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suíça</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Franco WIR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suriname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dólar do Suriname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DTH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ilhas Svalbard e Jan Mayen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suazilândia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lilangeni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SZL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">República Árabe da Síria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Libra síria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SYP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tadjiquistão</t>
-  </si>
-  <si>
-    <t xml:space="preserve">somoni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TJS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taiwan, Província da China</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Novo dólar de Taiwan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TWD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tanzânia, República Unida da</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Xelim da Tanzânia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TZS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Territórios Franceses do Sul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">República Tcheca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coroa checa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CZK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tailândia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">baht</t>
-  </si>
-  <si>
-    <t xml:space="preserve">THB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Timor Leste</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Togo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tokelau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tonga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tonga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trinidad e Tobago</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dólar de Trinidad e Tobago</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tunísia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dinar tunisino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Turcomenistão</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TMM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ilhas Turks e Caicos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Turquia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lira Turca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tuvalu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ucrânia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hryvnia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UAH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uruguai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peso uruguaio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UYU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peso uruguaio em Unidades Indexadas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uyi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vanuatu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vatu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VUV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cidade do Vaticano Estado da Santa Sé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Venezuela</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bolivar Venezuelano</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VEB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vietnã</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dong</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wallis e Futuna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iémen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rial do Iêmen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zâmbia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zimbábue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dólar do Zimbábue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZWD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lei Romeno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROL</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ouro</t>
   </si>
   <si>
     <t xml:space="preserve">XAU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iugoslávia</t>
   </si>
   <si>
     <t xml:space="preserve">Dinar Iugoslavo</t>
@@ -1966,11 +1969,11 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A158" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D155" activeCellId="0" sqref="D155"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A241" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A252" activeCellId="0" sqref="A252"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="18.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="18.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="25.54"/>
   </cols>
@@ -4284,22 +4287,22 @@
         <v>475</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>476</v>
+        <v>371</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>477</v>
+        <v>372</v>
       </c>
       <c r="D193" s="1"/>
     </row>
     <row r="194" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="C194" s="1" t="s">
         <v>478</v>
-      </c>
-      <c r="B194" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="C194" s="1" t="s">
-        <v>372</v>
       </c>
       <c r="D194" s="1"/>
     </row>
@@ -4308,16 +4311,16 @@
         <v>479</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>480</v>
+        <v>25</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>481</v>
+        <v>26</v>
       </c>
       <c r="D195" s="1"/>
     </row>
     <row r="196" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>25</v>
@@ -4329,19 +4332,19 @@
     </row>
     <row r="197" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>25</v>
+        <v>241</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>26</v>
+        <v>242</v>
       </c>
       <c r="D197" s="1"/>
     </row>
     <row r="198" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>241</v>
@@ -4353,25 +4356,25 @@
     </row>
     <row r="199" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>241</v>
+        <v>25</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>242</v>
+        <v>26</v>
       </c>
       <c r="D199" s="1"/>
     </row>
     <row r="200" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A200" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="C200" s="1" t="s">
         <v>486</v>
-      </c>
-      <c r="B200" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C200" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D200" s="1"/>
     </row>
@@ -4392,22 +4395,22 @@
         <v>490</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>491</v>
+        <v>187</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>492</v>
+        <v>188</v>
       </c>
       <c r="D202" s="1"/>
     </row>
     <row r="203" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A203" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="C203" s="1" t="s">
         <v>493</v>
-      </c>
-      <c r="B203" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C203" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="D203" s="1"/>
     </row>
@@ -4416,22 +4419,22 @@
         <v>494</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>495</v>
+        <v>74</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>496</v>
+        <v>75</v>
       </c>
       <c r="D204" s="1"/>
     </row>
     <row r="205" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="C205" s="1" t="s">
         <v>497</v>
-      </c>
-      <c r="B205" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C205" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="D205" s="1"/>
     </row>
@@ -4490,7 +4493,7 @@
       <c r="B210" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="C210" s="1" t="s">
+      <c r="C210" s="2" t="s">
         <v>512</v>
       </c>
       <c r="D210" s="1"/>
@@ -4502,7 +4505,7 @@
       <c r="B211" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C211" s="2" t="s">
+      <c r="C211" s="1" t="s">
         <v>515</v>
       </c>
       <c r="D211" s="1"/>
@@ -4548,28 +4551,28 @@
         <v>525</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>526</v>
+        <v>339</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>527</v>
+        <v>340</v>
       </c>
       <c r="D215" s="1"/>
     </row>
     <row r="216" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="s">
-        <v>528</v>
+        <v>79</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>339</v>
+        <v>526</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>340</v>
+        <v>527</v>
       </c>
       <c r="D216" s="1"/>
     </row>
     <row r="217" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="s">
-        <v>79</v>
+        <v>528</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>529</v>
@@ -4584,22 +4587,22 @@
         <v>531</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>532</v>
+        <v>94</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>533</v>
+        <v>95</v>
       </c>
       <c r="D218" s="1"/>
     </row>
     <row r="219" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A219" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="C219" s="1" t="s">
         <v>534</v>
-      </c>
-      <c r="B219" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C219" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="D219" s="1"/>
     </row>
@@ -4656,34 +4659,34 @@
         <v>547</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>548</v>
+        <v>241</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>549</v>
+        <v>242</v>
       </c>
       <c r="D224" s="1"/>
     </row>
     <row r="225" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A225" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>241</v>
+        <v>74</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>242</v>
+        <v>117</v>
       </c>
       <c r="D225" s="1"/>
     </row>
     <row r="226" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A226" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="C226" s="1" t="s">
         <v>551</v>
-      </c>
-      <c r="B226" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C226" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="D226" s="1"/>
     </row>
@@ -4704,46 +4707,46 @@
         <v>555</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>556</v>
+        <v>187</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>557</v>
+        <v>188</v>
       </c>
       <c r="D228" s="1"/>
     </row>
     <row r="229" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A229" s="1" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>187</v>
+        <v>74</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>188</v>
+        <v>75</v>
       </c>
       <c r="D229" s="1"/>
     </row>
     <row r="230" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>74</v>
+        <v>152</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>75</v>
+        <v>153</v>
       </c>
       <c r="D230" s="1"/>
     </row>
     <row r="231" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="C231" s="1" t="s">
         <v>560</v>
-      </c>
-      <c r="B231" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C231" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="D231" s="1"/>
     </row>
@@ -4776,34 +4779,34 @@
         <v>567</v>
       </c>
       <c r="B234" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C234" s="1" t="s">
         <v>568</v>
-      </c>
-      <c r="C234" s="1" t="s">
-        <v>569</v>
       </c>
       <c r="D234" s="1"/>
     </row>
     <row r="235" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A235" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>50</v>
+        <v>187</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>571</v>
+        <v>188</v>
       </c>
       <c r="D235" s="1"/>
     </row>
     <row r="236" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A236" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="C236" s="1" t="s">
         <v>572</v>
-      </c>
-      <c r="B236" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C236" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="D236" s="1"/>
     </row>
@@ -4812,22 +4815,22 @@
         <v>573</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>574</v>
+        <v>44</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>575</v>
+        <v>45</v>
       </c>
       <c r="D237" s="1"/>
     </row>
     <row r="238" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A238" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="C238" s="1" t="s">
         <v>576</v>
-      </c>
-      <c r="B238" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C238" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="D238" s="1"/>
     </row>
@@ -4845,19 +4848,19 @@
     </row>
     <row r="240" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A240" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B240" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="B240" s="1" t="s">
+      <c r="C240" s="1" t="s">
         <v>581</v>
-      </c>
-      <c r="C240" s="1" t="s">
-        <v>582</v>
       </c>
       <c r="D240" s="1"/>
     </row>
     <row r="241" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A241" s="1" t="s">
-        <v>79</v>
+        <v>582</v>
       </c>
       <c r="B241" s="1" t="s">
         <v>583</v>
@@ -4872,22 +4875,22 @@
         <v>585</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>586</v>
+        <v>241</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>587</v>
+        <v>242</v>
       </c>
       <c r="D242" s="1"/>
     </row>
     <row r="243" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A243" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="C243" s="1" t="s">
         <v>588</v>
-      </c>
-      <c r="B243" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="C243" s="1" t="s">
-        <v>242</v>
       </c>
       <c r="D243" s="1"/>
     </row>
@@ -4908,22 +4911,22 @@
         <v>592</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>593</v>
+        <v>418</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>594</v>
+        <v>419</v>
       </c>
       <c r="D245" s="1"/>
     </row>
     <row r="246" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="C246" s="1" t="s">
         <v>595</v>
-      </c>
-      <c r="B246" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="C246" s="1" t="s">
-        <v>419</v>
       </c>
       <c r="D246" s="1"/>
     </row>
@@ -4932,22 +4935,22 @@
         <v>596</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>597</v>
+        <v>360</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>598</v>
+        <v>360</v>
       </c>
       <c r="D247" s="1"/>
     </row>
     <row r="248" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="C248" s="1" t="s">
         <v>599</v>
-      </c>
-      <c r="B248" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="C248" s="1" t="s">
-        <v>360</v>
       </c>
       <c r="D248" s="1"/>
     </row>
@@ -4961,10 +4964,11 @@
       <c r="C249" s="1" t="s">
         <v>602</v>
       </c>
-      <c r="D249" s="1"/>
     </row>
     <row r="250" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A250" s="1"/>
+      <c r="A250" s="1" t="s">
+        <v>600</v>
+      </c>
       <c r="B250" s="1" t="s">
         <v>603</v>
       </c>
@@ -4973,7 +4977,9 @@
       </c>
     </row>
     <row r="251" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A251" s="1"/>
+      <c r="A251" s="1" t="s">
+        <v>605</v>
+      </c>
       <c r="B251" s="1" t="s">
         <v>605</v>
       </c>
@@ -4982,12 +4988,14 @@
       </c>
     </row>
     <row r="252" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A252" s="1"/>
+      <c r="A252" s="1" t="s">
+        <v>607</v>
+      </c>
       <c r="B252" s="1" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="18.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5184,7 +5192,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:D250"/>
+  <autoFilter ref="A1:D249"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>